<commit_message>
Applied css to profile page
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Project website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD9841-DE9B-4AC2-980E-E73C7109AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE9C113-0DD7-407C-BDB5-54F80A5022ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Address</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Parent_Phone_Number</t>
+  </si>
+  <si>
+    <t>Leave_Approved</t>
+  </si>
+  <si>
+    <t>Leave_Applied</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,10 +558,12 @@
     <col min="6" max="10" width="12.6328125" customWidth="1"/>
     <col min="11" max="11" width="8.6328125" customWidth="1"/>
     <col min="12" max="12" width="10.81640625" customWidth="1"/>
-    <col min="13" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="13" max="13" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -595,8 +603,14 @@
       <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>902634020041</v>
       </c>
@@ -636,8 +650,14 @@
       <c r="M2" t="s">
         <v>19</v>
       </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>781678351607</v>
       </c>
@@ -676,6 +696,12 @@
       </c>
       <c r="M3" t="s">
         <v>19</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added css for admin page
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMEN\Desktop\Project-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Project website\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6AAFBF-9FC0-4606-AA15-71B2191A26CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>ECE</t>
   </si>
@@ -136,12 +137,30 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>Peeyush Vatsi</t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>Bagdadi</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>ghi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -570,31 +589,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1"/>
-    <col min="6" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.90625" customWidth="1"/>
+    <col min="6" max="10" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6328125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="17" width="8.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11.21875" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" customWidth="1"/>
-    <col min="21" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="15" max="17" width="8.6328125" customWidth="1"/>
+    <col min="18" max="18" width="12.6328125" customWidth="1"/>
+    <col min="19" max="19" width="11.1796875" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" customWidth="1"/>
+    <col min="21" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -656,7 +675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>902634020041</v>
       </c>
@@ -718,7 +737,7 @@
         <v>44572</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>781678351607</v>
       </c>
@@ -777,12 +796,198 @@
         <v>44572</v>
       </c>
       <c r="T3" s="5">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>781678351607</v>
+      </c>
+      <c r="B4">
+        <v>19105008</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2">
+        <v>37358</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>9417298911</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>12345</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>545</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="5">
+        <v>44572</v>
+      </c>
+      <c r="T4" s="5">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>781678351607</v>
+      </c>
+      <c r="B5">
+        <v>19105030</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2">
+        <v>37358</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>9417298911</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>12345</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>545</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="5">
+        <v>44572</v>
+      </c>
+      <c r="T5" s="5">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>781678351607</v>
+      </c>
+      <c r="B6">
+        <v>19105015</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2">
+        <v>37358</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <v>9417298911</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>12345</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>545</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="5">
+        <v>44572</v>
+      </c>
+      <c r="T6" s="5">
         <v>44572</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Attached Database with Leave controllers
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Project website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMEN\Downloads\Project-website-master\Project-website-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6AAFBF-9FC0-4606-AA15-71B2191A26CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>ECE</t>
   </si>
@@ -58,9 +57,6 @@
     <t>7696046760</t>
   </si>
   <si>
-    <t>ansh chawla.bt19ece@pec.edu.out</t>
-  </si>
-  <si>
     <t>Anil Chawla</t>
   </si>
   <si>
@@ -100,12 +96,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>leave_approved</t>
-  </si>
-  <si>
-    <t>leave_applied</t>
-  </si>
-  <si>
     <t>on_leave</t>
   </si>
   <si>
@@ -115,24 +105,12 @@
     <t>room_number</t>
   </si>
   <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>visiting_address</t>
-  </si>
-  <si>
     <t>rg</t>
   </si>
   <si>
-    <t>gwdvd</t>
-  </si>
-  <si>
     <t>sfdbsb</t>
   </si>
   <si>
-    <t>sdvb</t>
-  </si>
-  <si>
     <t>start_date</t>
   </si>
   <si>
@@ -148,23 +126,74 @@
     <t>Bagdadi</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>ghi</t>
+    <t>mohabbat bin salman</t>
+  </si>
+  <si>
+    <t>Ravinder Nath</t>
+  </si>
+  <si>
+    <t>peeyushvatsi.bt19ece@pec.edu.out</t>
+  </si>
+  <si>
+    <t>anshchawla.bt19ece@pec.edu.out</t>
+  </si>
+  <si>
+    <t>harshkumar.bt19ece@pec.edu.out</t>
+  </si>
+  <si>
+    <t>raghavmittal.bt19ece@pec.edu.out</t>
+  </si>
+  <si>
+    <t>Bagdad, Iraq</t>
+  </si>
+  <si>
+    <t>Sangroor</t>
+  </si>
+  <si>
+    <t>Mandi</t>
+  </si>
+  <si>
+    <t>lateleave_date</t>
+  </si>
+  <si>
+    <t>longleave_reason</t>
+  </si>
+  <si>
+    <t>lateleave_address</t>
+  </si>
+  <si>
+    <t>longleave_address</t>
+  </si>
+  <si>
+    <t>lateleave_reason</t>
+  </si>
+  <si>
+    <t>lateleaves_sem</t>
+  </si>
+  <si>
+    <t>lateleaves_month</t>
+  </si>
+  <si>
+    <t>longleave_approved</t>
+  </si>
+  <si>
+    <t>longleave_applied</t>
+  </si>
+  <si>
+    <t>lateleave_approved</t>
+  </si>
+  <si>
+    <t>lateleave_applied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +217,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,10 +243,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -220,8 +258,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -589,97 +632,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="4" width="12.6328125" customWidth="1"/>
-    <col min="5" max="5" width="22.90625" customWidth="1"/>
-    <col min="6" max="10" width="12.6328125" customWidth="1"/>
-    <col min="11" max="11" width="8.6328125" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" customWidth="1"/>
-    <col min="13" max="13" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="17" width="8.6328125" customWidth="1"/>
-    <col min="18" max="18" width="12.6328125" customWidth="1"/>
-    <col min="19" max="19" width="11.1796875" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" customWidth="1"/>
-    <col min="21" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="15" max="16" width="8.6640625" customWidth="1"/>
+    <col min="18" max="19" width="8.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" customWidth="1"/>
+    <col min="21" max="21" width="9.33203125" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.21875" customWidth="1"/>
+    <col min="24" max="24" width="10.77734375" customWidth="1"/>
+    <col min="25" max="1020" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>38</v>
+      <c r="Y1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>902634020041</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -710,38 +779,59 @@
         <v>7</v>
       </c>
       <c r="L2">
-        <v>1234</v>
+        <v>5006</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
       <c r="O2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>516</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="5">
-        <v>44572</v>
+        <v>29</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
       </c>
       <c r="T2" s="5">
         <v>44572</v>
       </c>
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X2" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>781678351607</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -759,11 +849,11 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
       </c>
       <c r="J3">
         <v>9417298911</v>
@@ -772,10 +862,10 @@
         <v>7</v>
       </c>
       <c r="L3">
-        <v>12345</v>
+        <v>5031</v>
       </c>
       <c r="M3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -787,33 +877,54 @@
         <v>545</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="5">
-        <v>44572</v>
+        <v>29</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
       </c>
       <c r="T3" s="5">
         <v>44572</v>
       </c>
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X3" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>781678351607</v>
+        <v>681678351607</v>
       </c>
       <c r="B4">
         <v>19105008</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
-        <v>37358</v>
+        <v>36743</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -821,11 +932,11 @@
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>12</v>
+      <c r="H4" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J4">
         <v>9417298911</v>
@@ -834,13 +945,13 @@
         <v>7</v>
       </c>
       <c r="L4">
-        <v>12345</v>
+        <v>5008</v>
       </c>
       <c r="M4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
@@ -849,33 +960,54 @@
         <v>545</v>
       </c>
       <c r="Q4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="5">
-        <v>44572</v>
+        <v>29</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
       </c>
       <c r="T4" s="5">
         <v>44572</v>
       </c>
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X4" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>781678351607</v>
+        <v>581678351607</v>
       </c>
       <c r="B5">
         <v>19105030</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2">
-        <v>37358</v>
+        <v>36537</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -883,11 +1015,11 @@
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>12</v>
+      <c r="H5" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>9417298911</v>
@@ -896,13 +1028,13 @@
         <v>7</v>
       </c>
       <c r="L5">
-        <v>12345</v>
+        <v>5030</v>
       </c>
       <c r="M5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -911,33 +1043,54 @@
         <v>545</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="5">
-        <v>44572</v>
+        <v>29</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
       </c>
       <c r="T5" s="5">
         <v>44572</v>
       </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X5" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>781678351607</v>
+        <v>481678351607</v>
       </c>
       <c r="B6">
         <v>19105015</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2">
+        <v>37241</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" s="2">
-        <v>37358</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -945,11 +1098,11 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>12</v>
+      <c r="H6" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="J6">
         <v>9417298911</v>
@@ -958,13 +1111,13 @@
         <v>7</v>
       </c>
       <c r="L6">
-        <v>12345</v>
+        <v>5015</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" t="b">
         <v>0</v>
@@ -973,21 +1126,46 @@
         <v>545</v>
       </c>
       <c r="Q6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="5">
-        <v>44572</v>
+        <v>29</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
       </c>
       <c r="T6" s="5">
         <v>44572</v>
+      </c>
+      <c r="U6" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X6" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
added functionalities for admin
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMEN\Downloads\Project-website-master\Project-website-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMEN\OneDrive\Desktop\Project-website-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>ECE</t>
   </si>
@@ -123,12 +123,6 @@
     <t>Harsh</t>
   </si>
   <si>
-    <t>Bagdadi</t>
-  </si>
-  <si>
-    <t>mohabbat bin salman</t>
-  </si>
-  <si>
     <t>Ravinder Nath</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>raghavmittal.bt19ece@pec.edu.out</t>
   </si>
   <si>
-    <t>Bagdad, Iraq</t>
-  </si>
-  <si>
     <t>Sangroor</t>
   </si>
   <si>
@@ -184,6 +175,24 @@
   </si>
   <si>
     <t>lateleave_applied</t>
+  </si>
+  <si>
+    <t>Bathinda</t>
+  </si>
+  <si>
+    <t>Raghav</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>to_show_late</t>
+  </si>
+  <si>
+    <t>to_show_long</t>
   </si>
 </sst>
 </file>
@@ -633,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,7 +670,7 @@
     <col min="25" max="1020" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -702,31 +711,31 @@
         <v>25</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>30</v>
@@ -735,16 +744,22 @@
         <v>31</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>902634020041</v>
       </c>
@@ -785,7 +800,7 @@
         <v>13</v>
       </c>
       <c r="N2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="b">
         <v>0</v>
@@ -821,13 +836,19 @@
         <v>29</v>
       </c>
       <c r="Z2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="b">
         <v>0</v>
       </c>
+      <c r="AB2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>781678351607</v>
       </c>
@@ -850,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
@@ -871,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>545</v>
@@ -909,8 +930,14 @@
       <c r="AA3" t="b">
         <v>0</v>
       </c>
+      <c r="AB3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>681678351607</v>
       </c>
@@ -924,7 +951,7 @@
         <v>36743</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -933,10 +960,10 @@
         <v>11</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4">
         <v>9417298911</v>
@@ -992,8 +1019,14 @@
       <c r="AA4" t="b">
         <v>0</v>
       </c>
+      <c r="AB4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>581678351607</v>
       </c>
@@ -1007,7 +1040,7 @@
         <v>36537</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -1016,10 +1049,10 @@
         <v>11</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="J5">
         <v>9417298911</v>
@@ -1075,8 +1108,14 @@
       <c r="AA5" t="b">
         <v>0</v>
       </c>
+      <c r="AB5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>481678351607</v>
       </c>
@@ -1084,13 +1123,13 @@
         <v>19105015</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2">
         <v>37241</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -1099,10 +1138,10 @@
         <v>11</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="J6">
         <v>9417298911</v>
@@ -1156,6 +1195,12 @@
         <v>0</v>
       </c>
       <c r="AA6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new admin and more functionalitites
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>ECE</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>to_show_long</t>
+  </si>
+  <si>
+    <t>phone_number_temp</t>
+  </si>
+  <si>
+    <t>guardian_phone_number_long</t>
+  </si>
+  <si>
+    <t>guardian_phone_number_late</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Jyoti Kedia</t>
+  </si>
+  <si>
+    <t>Admin2</t>
   </si>
 </sst>
 </file>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,7 +688,7 @@
     <col min="25" max="1020" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="1" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -758,46 +776,55 @@
       <c r="AC1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>902634020041</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>881678351607</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>37272</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7015666589</v>
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="L2">
-        <v>5006</v>
+        <v>11223</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="N2" t="b">
         <v>0</v>
@@ -805,11 +832,11 @@
       <c r="O2" t="b">
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>516</v>
+      <c r="P2" t="s">
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -817,23 +844,23 @@
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2" s="5">
-        <v>44572</v>
+      <c r="T2" t="s">
+        <v>61</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="5">
-        <v>44572</v>
-      </c>
-      <c r="X2" s="5">
-        <v>44572</v>
+        <v>61</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" t="s">
+        <v>61</v>
       </c>
       <c r="Y2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="Z2" t="b">
         <v>0</v>
@@ -847,46 +874,55 @@
       <c r="AC2" t="b">
         <v>0</v>
       </c>
+      <c r="AD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>781678351607</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>281678351607</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2">
-        <v>37358</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>36</v>
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>9417298911</v>
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="L3">
-        <v>5031</v>
+        <v>11223</v>
       </c>
       <c r="M3" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -894,11 +930,11 @@
       <c r="O3" t="b">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>545</v>
+      <c r="P3" t="s">
+        <v>61</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -906,23 +942,23 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3" s="5">
-        <v>44572</v>
+      <c r="T3" t="s">
+        <v>61</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="5">
-        <v>44572</v>
-      </c>
-      <c r="X3" s="5">
-        <v>44572</v>
+        <v>61</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>61</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="Z3" t="b">
         <v>0</v>
@@ -936,8 +972,17 @@
       <c r="AC3" t="b">
         <v>0</v>
       </c>
+      <c r="AD3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>681678351607</v>
       </c>
@@ -1025,8 +1070,17 @@
       <c r="AC4" t="b">
         <v>0</v>
       </c>
+      <c r="AD4">
+        <v>6546</v>
+      </c>
+      <c r="AE4">
+        <v>6546</v>
+      </c>
+      <c r="AF4">
+        <v>6546</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>581678351607</v>
       </c>
@@ -1114,8 +1168,17 @@
       <c r="AC5" t="b">
         <v>0</v>
       </c>
+      <c r="AD5">
+        <v>6546</v>
+      </c>
+      <c r="AE5">
+        <v>6546</v>
+      </c>
+      <c r="AF5">
+        <v>6546</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>481678351607</v>
       </c>
@@ -1202,13 +1265,218 @@
       </c>
       <c r="AC6" t="b">
         <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>6546</v>
+      </c>
+      <c r="AE6">
+        <v>6546</v>
+      </c>
+      <c r="AF6">
+        <v>6546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>902634020041</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>37272</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>7015666589</v>
+      </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>5006</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>516</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5">
+        <v>44572</v>
+      </c>
+      <c r="U7" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X7" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>6546</v>
+      </c>
+      <c r="AE7">
+        <v>6546</v>
+      </c>
+      <c r="AF7">
+        <v>6546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>781678351607</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>37358</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>9417298911</v>
+      </c>
+      <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>5031</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>545</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
+        <v>44572</v>
+      </c>
+      <c r="U8" t="s">
+        <v>29</v>
+      </c>
+      <c r="V8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8" s="5">
+        <v>44572</v>
+      </c>
+      <c r="X8" s="5">
+        <v>44572</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>6546</v>
+      </c>
+      <c r="AE8">
+        <v>6546</v>
+      </c>
+      <c r="AF8">
+        <v>6546</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H7" r:id="rId1"/>
     <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H8" r:id="rId3"/>
     <hyperlink ref="H5" r:id="rId4"/>
     <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>

</xml_diff>